<commit_message>
Commiting Status, there is a circular import in the utils module that I need to resolve
</commit_message>
<xml_diff>
--- a/data/Obesity_Dataset.xlsx
+++ b/data/Obesity_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukastang/Documents/GitHub/Model_Interpretability/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01603F43-B9AB-2E42-A70F-0A3DD6D7121D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBB4122-1B73-BE4B-9FE6-20F3936746C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28480" windowHeight="10280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="obesity_dataset" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
     <t>More than 2 Liters</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>1-2 days per week</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>Obesity</t>
+  </si>
+  <si>
+    <t>No sports</t>
   </si>
 </sst>
 </file>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -76673,8 +76673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -76982,6 +76982,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A40"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:A4"/>
@@ -76989,13 +76996,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -77006,11 +77006,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13A32E9-EFF5-D44F-AAF2-897DAE7971F1}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -77284,7 +77289,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -77295,7 +77300,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -77306,7 +77311,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -77317,7 +77322,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -77328,7 +77333,7 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -77339,7 +77344,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -77350,7 +77355,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -77361,7 +77366,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -77372,7 +77377,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -77383,7 +77388,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -77394,7 +77399,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -77405,7 +77410,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -77416,7 +77421,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -77427,7 +77432,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -77438,7 +77443,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -77449,7 +77454,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -77460,11 +77465,12 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>